<commit_message>
require doc, schedule doc
终板需求文档V1.0，和初版的时间计划。
</commit_message>
<xml_diff>
--- a/misc/文档/crm-schedule.xlsx
+++ b/misc/文档/crm-schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="11880" windowHeight="6555" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="11880" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="taskList" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="96">
   <si>
     <t>一级菜单</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,9 +39,6 @@
   <si>
     <t>P2</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>P3</t>
   </si>
   <si>
     <t>P3</t>
@@ -142,54 +139,6 @@
     <t>系统管理</t>
   </si>
   <si>
-    <t>同行业务开通审批</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增承包区审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增加盟商审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>网点区域细分审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>网点删除审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>网点转让审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>快运补贴申请审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>网点派费提现审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>归属分拨中心调整审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>网点费率调整审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>加盟商物料费调整审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>二次申述审批</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>审批信息查询统计</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -198,42 +147,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>网点异常登记</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>网点异常反馈</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>网点异常查询</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>网点资料查询</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>物料费查询</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>费率查询</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>流程审批管理</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>我的工作列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>我的审批列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>H</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -242,35 +159,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>H</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>L</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>二期</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>二期</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>审批流程设置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>详细设计</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>DEMO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -306,129 +199,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>工作流引擎</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>审批流程</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>status</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>完成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>工作流引擎·后台实体·审批流程</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>L,B</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>L</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y,B</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y,B</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y，L</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>网点资料查询</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>报价单查询</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>审批信息综合查询</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>审批信息统计报表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页面根据</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1.demo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页面</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>文档进行开发</t>
-    </r>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -547,6 +322,142 @@
     </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>主界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求文档编写</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>计划编写</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进行中</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>主界面</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>L,Z</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y,Z</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y,Z</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户转移、分享、导出、导入</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>L,Z</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>联系人导出、导入</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户快速查询、高级查询</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>联系人快速查询、高级查询</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>行为快速查询、高级查询</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务快速查询、高级查询</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商机快速查询、高级查询</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件查询</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库备份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户查重</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户合并</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件新增、删除、下载</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>行为新增、修改、删除、查看</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务新增、修改、删除、查看</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商机新增、修改、删除、查看</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>联系人新增、修改、删除、查看</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户新增、修改、删除、查看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户复制</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>未开始</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -555,7 +466,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -951,7 +862,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1169,8 +1080,29 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1178,9 +1110,6 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1193,21 +1122,6 @@
     <xf numFmtId="0" fontId="22" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1217,7 +1131,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1547,18 +1461,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" style="43"/>
     <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="3" max="3" width="25.625" customWidth="1"/>
     <col min="4" max="4" width="8.5" style="43" customWidth="1"/>
     <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="23.875" customWidth="1"/>
@@ -1568,739 +1482,666 @@
     <col min="10" max="10" width="37.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29.25" customHeight="1">
       <c r="A1" s="75"/>
-      <c r="B1" s="103" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="103"/>
+      <c r="B1" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="98"/>
       <c r="D1" s="54"/>
       <c r="E1" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="G1" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="100"/>
+      <c r="I1" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="92" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="93"/>
-      <c r="I1" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="55" t="s">
-        <v>23</v>
-      </c>
       <c r="K1" s="90" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99" t="s">
-        <v>69</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A2" s="93" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="71" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="57"/>
-      <c r="E2" s="58" t="s">
-        <v>62</v>
-      </c>
+      <c r="E2" s="58"/>
       <c r="F2" s="59"/>
       <c r="G2" s="60"/>
       <c r="H2" s="61">
-        <v>41425</v>
+        <v>41506</v>
       </c>
       <c r="I2" s="73"/>
-      <c r="J2" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="99"/>
+      <c r="J2" s="74"/>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="93"/>
       <c r="B3" s="71"/>
       <c r="C3" s="89" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D3" s="57"/>
       <c r="E3" s="58"/>
       <c r="F3" s="64" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G3" s="60"/>
       <c r="H3" s="61"/>
       <c r="I3" s="73"/>
-      <c r="J3" s="63" t="s">
-        <v>77</v>
-      </c>
+      <c r="J3" s="63"/>
       <c r="K3" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="99"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A4" s="93"/>
       <c r="B4" s="71"/>
       <c r="C4" s="89" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="64" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G4" s="60"/>
       <c r="H4" s="61"/>
       <c r="I4" s="73"/>
-      <c r="J4" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" s="91" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="99"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A5" s="93"/>
       <c r="B5" s="71" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C5" s="72"/>
       <c r="D5" s="57"/>
-      <c r="E5" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="64" t="s">
-        <v>79</v>
-      </c>
+      <c r="E5" s="58"/>
+      <c r="F5" s="64"/>
       <c r="G5" s="60"/>
-      <c r="H5" s="62">
-        <v>41439</v>
-      </c>
+      <c r="H5" s="62"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="K5" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="101" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="98" t="s">
-        <v>67</v>
+      <c r="J5" s="59"/>
+      <c r="K5" s="49"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="104" t="s">
+        <v>40</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
-      <c r="E6" s="63" t="s">
-        <v>53</v>
-      </c>
+      <c r="E6" s="63"/>
       <c r="F6" s="64"/>
-      <c r="G6" s="65">
-        <v>41411</v>
-      </c>
-      <c r="H6" s="65">
-        <v>41421</v>
-      </c>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
       <c r="I6" s="73"/>
-      <c r="J6" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A7" s="102"/>
-      <c r="B7" s="98"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="96"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="38"/>
-      <c r="E7" s="26"/>
+      <c r="E7" s="26" t="s">
+        <v>68</v>
+      </c>
       <c r="F7" s="64" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="73"/>
-      <c r="J7" s="63" t="s">
-        <v>73</v>
-      </c>
+      <c r="J7" s="63"/>
       <c r="K7" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="102"/>
-      <c r="B8" s="98"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="39" customFormat="1">
+      <c r="A8" s="96"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="38"/>
-      <c r="E8" s="26"/>
+      <c r="E8" s="26" t="s">
+        <v>68</v>
+      </c>
       <c r="F8" s="64" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
       <c r="I8" s="73"/>
-      <c r="J8" s="63" t="s">
-        <v>73</v>
-      </c>
+      <c r="J8" s="63"/>
       <c r="K8" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="102"/>
-      <c r="B9" s="98"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="39" customFormat="1">
+      <c r="A9" s="96"/>
+      <c r="B9" s="104"/>
       <c r="C9" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="64" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="73"/>
-      <c r="J9" s="63" t="s">
-        <v>73</v>
-      </c>
+      <c r="J9" s="63"/>
       <c r="K9" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="102"/>
-      <c r="B10" s="98"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="43" customFormat="1">
+      <c r="A10" s="96"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="38" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="63"/>
       <c r="F10" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
+        <v>66</v>
+      </c>
+      <c r="G10" s="67">
+        <v>41500</v>
+      </c>
+      <c r="H10" s="67">
+        <v>41503</v>
+      </c>
       <c r="I10" s="73"/>
-      <c r="J10" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K10" s="91" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="100" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="98" t="s">
-        <v>65</v>
+      <c r="J10" s="63"/>
+      <c r="K10" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="43" customFormat="1">
+      <c r="A11" s="94" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="104" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="63"/>
       <c r="F11" s="64"/>
       <c r="G11" s="65">
-        <v>41425</v>
+        <v>41499</v>
       </c>
       <c r="H11" s="65">
-        <v>41435</v>
+        <v>41500</v>
       </c>
       <c r="I11" s="73"/>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="1:11" s="40" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="100"/>
-      <c r="B12" s="98"/>
+    <row r="12" spans="1:11" s="40" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A12" s="94"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="38" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D12" s="38"/>
       <c r="E12" s="63" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="F12" s="64" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
       <c r="I12" s="73"/>
-      <c r="J12" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="K12" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A13" s="100"/>
-      <c r="B13" s="95" t="s">
-        <v>68</v>
+      <c r="J12" s="63"/>
+      <c r="K12" s="49"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="94"/>
+      <c r="B13" s="101" t="s">
+        <v>41</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="64"/>
       <c r="G13" s="65">
-        <v>41425</v>
+        <v>41476</v>
       </c>
       <c r="H13" s="65">
-        <v>41439</v>
+        <v>41483</v>
       </c>
       <c r="I13" s="73"/>
       <c r="J13" s="26"/>
     </row>
-    <row r="14" spans="1:11" s="39" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="100"/>
-      <c r="B14" s="96"/>
+    <row r="14" spans="1:11" s="39" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A14" s="94"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="38" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="D14" s="38"/>
       <c r="E14" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F14" s="64" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="67"/>
       <c r="I14" s="73"/>
-      <c r="J14" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="39" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="100"/>
-      <c r="B15" s="96"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="39" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A15" s="94"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="38" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="D15" s="38"/>
       <c r="E15" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F15" s="64" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="67"/>
       <c r="I15" s="73"/>
-      <c r="J15" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K15" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="39" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="100"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="38" t="s">
-        <v>32</v>
-      </c>
+      <c r="J15" s="63"/>
+      <c r="K15" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="43" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A16" s="94"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="67"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="65">
+        <v>41476</v>
+      </c>
+      <c r="H16" s="65">
+        <v>41486</v>
+      </c>
       <c r="I16" s="73"/>
-      <c r="J16" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K16" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A17" s="100"/>
-      <c r="B17" s="96"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="49"/>
+    </row>
+    <row r="17" spans="1:11" s="39" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A17" s="94"/>
+      <c r="B17" s="102"/>
       <c r="C17" s="38" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="D17" s="38"/>
       <c r="E17" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F17" s="64" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="67"/>
       <c r="I17" s="73"/>
-      <c r="J17" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K17" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A18" s="100"/>
-      <c r="B18" s="96"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="94"/>
+      <c r="B18" s="102"/>
       <c r="C18" s="38" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D18" s="38"/>
       <c r="E18" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F18" s="64" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G18" s="26"/>
       <c r="H18" s="67"/>
       <c r="I18" s="73"/>
-      <c r="J18" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A19" s="100"/>
-      <c r="B19" s="96"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="94"/>
+      <c r="B19" s="102"/>
       <c r="C19" s="38" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F19" s="64" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G19" s="26"/>
       <c r="H19" s="67"/>
       <c r="I19" s="73"/>
-      <c r="J19" s="63" t="s">
+      <c r="J19" s="63"/>
+      <c r="K19" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="94"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65">
+        <v>41483</v>
+      </c>
+      <c r="H20" s="65">
+        <v>41489</v>
+      </c>
+      <c r="I20" s="73"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="49"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="94"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="38" t="s">
         <v>73</v>
-      </c>
-      <c r="K19" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A20" s="100"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K20" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A21" s="100"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="38" t="s">
-        <v>36</v>
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F21" s="64" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G21" s="26"/>
       <c r="H21" s="67"/>
       <c r="I21" s="73"/>
-      <c r="J21" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K21" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="100"/>
-      <c r="B22" s="96"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="43" customFormat="1">
+      <c r="A22" s="94"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="38" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="D22" s="38"/>
       <c r="E22" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F22" s="64" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G22" s="26"/>
       <c r="H22" s="67"/>
       <c r="I22" s="73"/>
-      <c r="J22" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K22" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="100"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="38" t="s">
-        <v>38</v>
-      </c>
+      <c r="J22" s="63"/>
+      <c r="K22" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="43" customFormat="1">
+      <c r="A23" s="94"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="38"/>
-      <c r="E23" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="67"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65">
+        <v>41489</v>
+      </c>
+      <c r="H23" s="65">
+        <v>41496</v>
+      </c>
       <c r="I23" s="73"/>
-      <c r="J23" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K23" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="100"/>
-      <c r="B24" s="96"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="49"/>
+    </row>
+    <row r="24" spans="1:11" s="43" customFormat="1">
+      <c r="A24" s="94"/>
+      <c r="B24" s="102"/>
       <c r="C24" s="38" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D24" s="38"/>
       <c r="E24" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F24" s="64" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G24" s="26"/>
       <c r="H24" s="67"/>
       <c r="I24" s="73"/>
-      <c r="J24" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K24" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="100"/>
-      <c r="B25" s="96"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="43" customFormat="1">
+      <c r="A25" s="94"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="38" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="26" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F25" s="64" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="67"/>
       <c r="I25" s="73"/>
-      <c r="J25" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K25" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A26" s="100"/>
-      <c r="B26" s="97"/>
-      <c r="C26" s="38" t="s">
-        <v>41</v>
-      </c>
+      <c r="J25" s="63"/>
+      <c r="K25" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="94"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="38"/>
       <c r="E26" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="64" t="s">
-        <v>81</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F26" s="64"/>
       <c r="G26" s="26"/>
       <c r="H26" s="67"/>
       <c r="I26" s="73"/>
-      <c r="J26" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="100"/>
-      <c r="B27" s="95" t="s">
-        <v>42</v>
+      <c r="J26" s="63"/>
+      <c r="K26" s="49"/>
+    </row>
+    <row r="27" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A27" s="94"/>
+      <c r="B27" s="101" t="s">
+        <v>29</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="64"/>
       <c r="G27" s="65">
-        <v>41441</v>
+        <v>41487</v>
       </c>
       <c r="H27" s="65">
-        <v>41446</v>
+        <v>41498</v>
       </c>
       <c r="I27" s="66"/>
       <c r="J27" s="63"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A28" s="100"/>
-      <c r="B28" s="96"/>
+    <row r="28" spans="1:11">
+      <c r="A28" s="94"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="38" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="26" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="F28" s="64" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G28" s="26"/>
       <c r="H28" s="67"/>
       <c r="I28" s="73"/>
-      <c r="J28" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K28" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A29" s="100"/>
-      <c r="B29" s="97"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="94"/>
+      <c r="B29" s="103"/>
       <c r="C29" s="38" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D29" s="38"/>
       <c r="E29" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="64"/>
+        <v>80</v>
+      </c>
+      <c r="F29" s="64" t="s">
+        <v>72</v>
+      </c>
       <c r="G29" s="26"/>
       <c r="H29" s="67"/>
       <c r="I29" s="73"/>
-      <c r="J29" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="K29" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A30" s="100"/>
-      <c r="B30" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="65">
-        <v>41456</v>
-      </c>
-      <c r="H30" s="65">
-        <v>41465</v>
-      </c>
-      <c r="I30" s="66"/>
-      <c r="J30" s="26"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A31" s="100"/>
-      <c r="B31" s="96"/>
-      <c r="C31" s="38" t="s">
-        <v>44</v>
-      </c>
+      <c r="J29" s="63"/>
+      <c r="K29" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="43" customFormat="1">
+      <c r="A30" s="94"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="38"/>
+      <c r="E30" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="26"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="73"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="43" customFormat="1">
+      <c r="A31" s="94"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="38"/>
-      <c r="E31" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="26"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="26"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A32" s="100"/>
-      <c r="B32" s="96"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="67">
+        <v>41499</v>
+      </c>
+      <c r="H31" s="67">
+        <v>41504</v>
+      </c>
+      <c r="I31" s="73"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="49"/>
+    </row>
+    <row r="32" spans="1:11" s="43" customFormat="1">
+      <c r="A32" s="94"/>
+      <c r="B32" s="91"/>
       <c r="C32" s="38" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="D32" s="38"/>
       <c r="E32" s="26" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F32" s="64" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G32" s="26"/>
       <c r="H32" s="67"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="26"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A33" s="100"/>
-      <c r="B33" s="97"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="43" customFormat="1">
+      <c r="A33" s="94"/>
+      <c r="B33" s="91"/>
       <c r="C33" s="38" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="D33" s="38"/>
       <c r="E33" s="26" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F33" s="64" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G33" s="26"/>
       <c r="H33" s="67"/>
-      <c r="I33" s="68"/>
+      <c r="I33" s="73"/>
       <c r="J33" s="63"/>
-    </row>
-    <row r="34" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="100"/>
-      <c r="B34" s="95" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
+      <c r="K33" s="108" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="94"/>
+      <c r="B34" s="101" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="26"/>
       <c r="F34" s="64"/>
       <c r="G34" s="65"/>
@@ -2308,336 +2149,368 @@
       <c r="I34" s="66"/>
       <c r="J34" s="26"/>
     </row>
-    <row r="35" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="100"/>
-      <c r="B35" s="96"/>
+    <row r="35" spans="1:11">
+      <c r="A35" s="94"/>
+      <c r="B35" s="102"/>
       <c r="C35" s="38" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D35" s="38"/>
       <c r="E35" s="26" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F35" s="64"/>
       <c r="G35" s="26"/>
-      <c r="H35" s="69"/>
+      <c r="H35" s="67"/>
       <c r="I35" s="66"/>
       <c r="J35" s="26"/>
     </row>
-    <row r="36" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="100"/>
-      <c r="B36" s="96"/>
+    <row r="36" spans="1:11">
+      <c r="A36" s="94"/>
+      <c r="B36" s="102"/>
       <c r="C36" s="38" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="D36" s="38"/>
       <c r="E36" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="70"/>
+        <v>65</v>
+      </c>
+      <c r="F36" s="64"/>
       <c r="G36" s="26"/>
-      <c r="H36" s="69"/>
+      <c r="H36" s="67"/>
       <c r="I36" s="66"/>
       <c r="J36" s="26"/>
     </row>
-    <row r="37" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="100"/>
-      <c r="B37" s="96"/>
+    <row r="37" spans="1:11">
+      <c r="A37" s="94"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="38" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D37" s="38"/>
       <c r="E37" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" s="70"/>
+        <v>65</v>
+      </c>
+      <c r="F37" s="64"/>
       <c r="G37" s="26"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="26"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A38" s="100"/>
-      <c r="B38" s="97"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="68"/>
+      <c r="J37" s="63"/>
+    </row>
+    <row r="38" spans="1:11" s="43" customFormat="1">
+      <c r="A38" s="94"/>
+      <c r="B38" s="91"/>
       <c r="C38" s="38" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D38" s="38"/>
       <c r="E38" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="G38" s="65">
-        <v>41449</v>
-      </c>
-      <c r="H38" s="65">
-        <v>41453</v>
-      </c>
-      <c r="I38" s="66"/>
-      <c r="J38" s="26"/>
-    </row>
-    <row r="39" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="100"/>
-      <c r="B39" s="95" t="s">
-        <v>50</v>
+        <v>93</v>
+      </c>
+      <c r="F38" s="64"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="63"/>
+    </row>
+    <row r="39" spans="1:11" s="42" customFormat="1">
+      <c r="A39" s="94"/>
+      <c r="B39" s="101" t="s">
+        <v>45</v>
       </c>
       <c r="C39" s="38"/>
       <c r="D39" s="38"/>
-      <c r="E39" s="63"/>
+      <c r="E39" s="26"/>
       <c r="F39" s="64"/>
-      <c r="G39" s="65">
-        <v>41439</v>
-      </c>
-      <c r="H39" s="65">
-        <v>41446</v>
-      </c>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
       <c r="I39" s="66"/>
-      <c r="J39" s="63"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A40" s="100"/>
-      <c r="B40" s="96"/>
-      <c r="C40" s="38" t="s">
-        <v>51</v>
-      </c>
+      <c r="J39" s="26"/>
+    </row>
+    <row r="40" spans="1:11" s="41" customFormat="1">
+      <c r="A40" s="94"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="38"/>
       <c r="D40" s="38"/>
-      <c r="E40" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="G40" s="65"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="73"/>
-      <c r="J40" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="K40" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A41" s="100"/>
-      <c r="B41" s="97"/>
-      <c r="C41" s="38" t="s">
-        <v>52</v>
-      </c>
+      <c r="E40" s="26"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="26"/>
+    </row>
+    <row r="41" spans="1:11" s="41" customFormat="1">
+      <c r="A41" s="94"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="38"/>
       <c r="D41" s="38"/>
-      <c r="E41" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="F41" s="64" t="s">
-        <v>81</v>
-      </c>
+      <c r="E41" s="26"/>
+      <c r="F41" s="70"/>
       <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="73"/>
-      <c r="J41" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="K41" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="47"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="50"/>
-      <c r="H42" s="51"/>
-    </row>
-    <row r="43" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="47"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="F43" s="50"/>
-    </row>
-    <row r="44" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="47"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="F44" s="50"/>
-    </row>
-    <row r="45" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="47"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="F45" s="50"/>
-    </row>
-    <row r="46" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="47"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="F46" s="50"/>
-    </row>
-    <row r="47" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H41" s="69"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="26"/>
+    </row>
+    <row r="42" spans="1:11" s="43" customFormat="1">
+      <c r="A42" s="94"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="66"/>
+      <c r="J42" s="26"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="94"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="26"/>
+    </row>
+    <row r="44" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A44" s="94"/>
+      <c r="B44" s="101" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="63"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="94"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="65"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="94"/>
+      <c r="B46" s="103"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="73"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+    </row>
+    <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="B47" s="47"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
+      <c r="E47" s="49"/>
       <c r="F47" s="50"/>
-    </row>
-    <row r="48" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H47" s="51"/>
+    </row>
+    <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="B48" s="47"/>
       <c r="C48" s="45"/>
       <c r="D48" s="45"/>
       <c r="F48" s="50"/>
     </row>
-    <row r="49" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:8" s="48" customFormat="1">
       <c r="B49" s="47"/>
       <c r="C49" s="45"/>
       <c r="D49" s="45"/>
       <c r="F49" s="50"/>
     </row>
-    <row r="50" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:8" s="48" customFormat="1">
       <c r="B50" s="47"/>
-      <c r="E50" s="49"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
       <c r="F50" s="50"/>
-      <c r="H50" s="52"/>
-    </row>
-    <row r="51" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="51" spans="2:8" s="48" customFormat="1">
       <c r="B51" s="47"/>
       <c r="C51" s="45"/>
       <c r="D51" s="45"/>
       <c r="F51" s="50"/>
     </row>
-    <row r="52" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:8" s="48" customFormat="1">
       <c r="B52" s="47"/>
       <c r="C52" s="45"/>
       <c r="D52" s="45"/>
       <c r="F52" s="50"/>
     </row>
-    <row r="53" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:8" s="48" customFormat="1">
       <c r="B53" s="47"/>
       <c r="C53" s="45"/>
       <c r="D53" s="45"/>
-      <c r="E53" s="49"/>
       <c r="F53" s="50"/>
-      <c r="H53" s="52"/>
-    </row>
-    <row r="54" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="54" spans="2:8" s="48" customFormat="1">
       <c r="B54" s="47"/>
       <c r="C54" s="45"/>
       <c r="D54" s="45"/>
-      <c r="E54" s="49"/>
       <c r="F54" s="50"/>
     </row>
-    <row r="55" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:8" s="48" customFormat="1">
       <c r="B55" s="47"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
+      <c r="E55" s="49"/>
       <c r="F55" s="50"/>
-    </row>
-    <row r="56" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H55" s="52"/>
+    </row>
+    <row r="56" spans="2:8" s="48" customFormat="1">
       <c r="B56" s="47"/>
       <c r="C56" s="45"/>
       <c r="D56" s="45"/>
       <c r="F56" s="50"/>
     </row>
-    <row r="57" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:8" s="48" customFormat="1">
       <c r="B57" s="47"/>
       <c r="C57" s="45"/>
       <c r="D57" s="45"/>
       <c r="F57" s="50"/>
     </row>
-    <row r="58" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:8" s="48" customFormat="1">
       <c r="B58" s="47"/>
       <c r="C58" s="45"/>
       <c r="D58" s="45"/>
+      <c r="E58" s="49"/>
       <c r="F58" s="50"/>
-    </row>
-    <row r="59" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H58" s="52"/>
+    </row>
+    <row r="59" spans="2:8" s="48" customFormat="1">
       <c r="B59" s="47"/>
       <c r="C59" s="45"/>
       <c r="D59" s="45"/>
+      <c r="E59" s="49"/>
       <c r="F59" s="50"/>
     </row>
-    <row r="60" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B60" s="94"/>
+    <row r="60" spans="2:8" s="48" customFormat="1">
+      <c r="B60" s="47"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
       <c r="F60" s="50"/>
-      <c r="H60" s="51"/>
-    </row>
-    <row r="61" spans="2:8" s="48" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B61" s="94"/>
-    </row>
-    <row r="62" spans="2:8" s="48" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B62" s="94"/>
-    </row>
-    <row r="63" spans="2:8" s="48" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B63" s="94"/>
-    </row>
-    <row r="64" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B64" s="94"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
+    </row>
+    <row r="61" spans="2:8" s="48" customFormat="1">
+      <c r="B61" s="47"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="45"/>
+      <c r="F61" s="50"/>
+    </row>
+    <row r="62" spans="2:8" s="48" customFormat="1">
+      <c r="B62" s="47"/>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="F62" s="50"/>
+    </row>
+    <row r="63" spans="2:8" s="48" customFormat="1">
+      <c r="B63" s="47"/>
+      <c r="C63" s="45"/>
+      <c r="D63" s="45"/>
+      <c r="F63" s="50"/>
+    </row>
+    <row r="64" spans="2:8" s="48" customFormat="1">
+      <c r="B64" s="47"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="45"/>
       <c r="F64" s="50"/>
-      <c r="H64" s="53"/>
-    </row>
-    <row r="65" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B65" s="94"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
-    </row>
-    <row r="66" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B66" s="94"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-    </row>
-    <row r="67" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B67" s="94"/>
-      <c r="C67" s="49"/>
-      <c r="D67" s="49"/>
-    </row>
-    <row r="68" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B68" s="94"/>
-      <c r="C68" s="49"/>
-      <c r="D68" s="49"/>
-      <c r="F68" s="50"/>
-      <c r="H68" s="53"/>
-    </row>
-    <row r="69" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B69" s="94"/>
+    </row>
+    <row r="65" spans="2:8" s="48" customFormat="1">
+      <c r="B65" s="97"/>
+      <c r="F65" s="50"/>
+      <c r="H65" s="51"/>
+    </row>
+    <row r="66" spans="2:8" s="48" customFormat="1" ht="18.75" customHeight="1">
+      <c r="B66" s="97"/>
+    </row>
+    <row r="67" spans="2:8" s="48" customFormat="1" ht="17.25" customHeight="1">
+      <c r="B67" s="97"/>
+    </row>
+    <row r="68" spans="2:8" s="48" customFormat="1" ht="26.25" customHeight="1">
+      <c r="B68" s="97"/>
+    </row>
+    <row r="69" spans="2:8" s="48" customFormat="1">
+      <c r="B69" s="97"/>
       <c r="C69" s="49"/>
       <c r="D69" s="49"/>
-    </row>
-    <row r="70" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B70" s="94"/>
+      <c r="F69" s="50"/>
+      <c r="H69" s="53"/>
+    </row>
+    <row r="70" spans="2:8" s="48" customFormat="1">
+      <c r="B70" s="97"/>
       <c r="C70" s="49"/>
       <c r="D70" s="49"/>
     </row>
-    <row r="71" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B71" s="94"/>
+    <row r="71" spans="2:8" s="48" customFormat="1">
+      <c r="B71" s="97"/>
       <c r="C71" s="49"/>
       <c r="D71" s="49"/>
     </row>
-    <row r="72" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B72" s="94"/>
+    <row r="72" spans="2:8" s="48" customFormat="1">
+      <c r="B72" s="97"/>
       <c r="C72" s="49"/>
       <c r="D72" s="49"/>
     </row>
-    <row r="73" spans="2:8" s="48" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B73" s="94"/>
+    <row r="73" spans="2:8" s="48" customFormat="1">
+      <c r="B73" s="97"/>
       <c r="C73" s="49"/>
       <c r="D73" s="49"/>
+      <c r="F73" s="50"/>
+      <c r="H73" s="53"/>
+    </row>
+    <row r="74" spans="2:8" s="48" customFormat="1">
+      <c r="B74" s="97"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="49"/>
+    </row>
+    <row r="75" spans="2:8" s="48" customFormat="1">
+      <c r="B75" s="97"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="49"/>
+    </row>
+    <row r="76" spans="2:8" s="48" customFormat="1">
+      <c r="B76" s="97"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="49"/>
+    </row>
+    <row r="77" spans="2:8" s="48" customFormat="1">
+      <c r="B77" s="97"/>
+      <c r="C77" s="49"/>
+      <c r="D77" s="49"/>
+    </row>
+    <row r="78" spans="2:8" s="48" customFormat="1">
+      <c r="B78" s="97"/>
+      <c r="C78" s="49"/>
+      <c r="D78" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A11:A41"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B68:B73"/>
-    <mergeCell ref="B1:C1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="B39:B43"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B13:B26"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A11:A46"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2653,10 +2526,10 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
@@ -2666,36 +2539,36 @@
     <col min="11" max="20" width="3.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="144.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="104" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="104" t="s">
-        <v>16</v>
+    <row r="1" spans="1:20" ht="144.75" customHeight="1">
+      <c r="A1" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="105" t="s">
+        <v>15</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="F1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="34" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="J1" s="35" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>11</v>
       </c>
       <c r="K1" s="85"/>
       <c r="L1" s="36"/>
@@ -2708,9 +2581,9 @@
       <c r="S1" s="36"/>
       <c r="T1" s="36"/>
     </row>
-    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="104"/>
-      <c r="B2" s="104"/>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
       <c r="C2" s="14"/>
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
@@ -2730,12 +2603,12 @@
       <c r="S2" s="19"/>
       <c r="T2" s="19"/>
     </row>
-    <row r="3" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" ht="13.5" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>1</v>
@@ -2779,12 +2652,12 @@
       <c r="S3" s="10"/>
       <c r="T3" s="8"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20">
       <c r="A4" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>1</v>
@@ -2828,12 +2701,12 @@
       <c r="S4" s="10"/>
       <c r="T4" s="8"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20">
       <c r="A5" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>1</v>
@@ -2877,12 +2750,12 @@
       <c r="S5" s="10"/>
       <c r="T5" s="8"/>
     </row>
-    <row r="6" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" ht="13.5" customHeight="1">
       <c r="A6" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C6" s="44" t="s">
         <v>1</v>
@@ -2926,12 +2799,12 @@
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20">
       <c r="A7" s="16" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>3</v>
@@ -2975,12 +2848,12 @@
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" ht="13.5" customHeight="1">
       <c r="A8" s="86" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>1</v>
@@ -3024,12 +2897,12 @@
       <c r="S8" s="10"/>
       <c r="T8" s="8"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20">
       <c r="A9" s="86" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>1</v>
@@ -3073,12 +2946,12 @@
       <c r="S9" s="10"/>
       <c r="T9" s="8"/>
     </row>
-    <row r="10" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" ht="13.5" customHeight="1">
       <c r="A10" s="86" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>1</v>
@@ -3122,12 +2995,12 @@
       <c r="S10" s="10"/>
       <c r="T10" s="8"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20">
       <c r="A11" s="86" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>1</v>
@@ -3171,12 +3044,12 @@
       <c r="S11" s="10"/>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20">
       <c r="A12" s="86" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="C12" s="23" t="s">
         <v>1</v>
@@ -3220,12 +3093,12 @@
       <c r="S12" s="10"/>
       <c r="T12" s="8"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20">
       <c r="A13" s="86" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>1</v>
@@ -3269,7 +3142,7 @@
       <c r="S13" s="10"/>
       <c r="T13" s="8"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20">
       <c r="A14" s="86"/>
       <c r="B14" s="38"/>
       <c r="C14" s="23"/>
@@ -3291,12 +3164,10 @@
       <c r="S14" s="10"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20">
       <c r="A15" s="86"/>
       <c r="B15" s="38"/>
-      <c r="C15" s="23" t="s">
-        <v>1</v>
-      </c>
+      <c r="C15" s="23"/>
       <c r="D15" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3336,12 +3207,10 @@
       <c r="S15" s="10"/>
       <c r="T15" s="8"/>
     </row>
-    <row r="16" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" ht="13.5" customHeight="1">
       <c r="A16" s="86"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="21" t="s">
-        <v>1</v>
-      </c>
+      <c r="C16" s="21"/>
       <c r="D16" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3381,12 +3250,10 @@
       <c r="S16" s="10"/>
       <c r="T16" s="8"/>
     </row>
-    <row r="17" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" ht="13.5" customHeight="1">
       <c r="A17" s="86"/>
       <c r="B17" s="38"/>
-      <c r="C17" s="21" t="s">
-        <v>1</v>
-      </c>
+      <c r="C17" s="21"/>
       <c r="D17" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3426,12 +3293,10 @@
       <c r="S17" s="10"/>
       <c r="T17" s="8"/>
     </row>
-    <row r="18" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" ht="13.5" customHeight="1">
       <c r="A18" s="86"/>
       <c r="B18" s="38"/>
-      <c r="C18" s="21" t="s">
-        <v>1</v>
-      </c>
+      <c r="C18" s="21"/>
       <c r="D18" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3471,12 +3336,10 @@
       <c r="S18" s="10"/>
       <c r="T18" s="8"/>
     </row>
-    <row r="19" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" ht="13.5" customHeight="1">
       <c r="A19" s="86"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="21" t="s">
-        <v>1</v>
-      </c>
+      <c r="C19" s="21"/>
       <c r="D19" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3516,12 +3379,10 @@
       <c r="S19" s="10"/>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" ht="13.5" customHeight="1">
       <c r="A20" s="86"/>
       <c r="B20" s="38"/>
-      <c r="C20" s="21" t="s">
-        <v>1</v>
-      </c>
+      <c r="C20" s="21"/>
       <c r="D20" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3561,11 +3422,15 @@
       <c r="S20" s="10"/>
       <c r="T20" s="8"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A21" s="22"/>
-      <c r="B21" s="38"/>
+    <row r="21" spans="1:20">
+      <c r="A21" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>62</v>
+      </c>
       <c r="C21" s="23" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" s="13">
         <f t="shared" si="3"/>
@@ -3606,12 +3471,10 @@
       <c r="S21" s="10"/>
       <c r="T21" s="8"/>
     </row>
-    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" ht="15" customHeight="1">
       <c r="A22" s="22"/>
       <c r="B22" s="76"/>
-      <c r="C22" s="23" t="s">
-        <v>5</v>
-      </c>
+      <c r="C22" s="23"/>
       <c r="D22" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3651,12 +3514,10 @@
       <c r="S22" s="10"/>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" ht="13.5" customHeight="1">
       <c r="A23" s="87"/>
       <c r="B23" s="38"/>
-      <c r="C23" s="21" t="s">
-        <v>5</v>
-      </c>
+      <c r="C23" s="21"/>
       <c r="D23" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3696,12 +3557,10 @@
       <c r="S23" s="10"/>
       <c r="T23" s="8"/>
     </row>
-    <row r="24" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" ht="13.5" customHeight="1">
       <c r="A24" s="87"/>
       <c r="B24" s="38"/>
-      <c r="C24" s="21" t="s">
-        <v>5</v>
-      </c>
+      <c r="C24" s="21"/>
       <c r="D24" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3741,12 +3600,10 @@
       <c r="S24" s="10"/>
       <c r="T24" s="8"/>
     </row>
-    <row r="25" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" ht="13.5" customHeight="1">
       <c r="A25" s="87"/>
       <c r="B25" s="38"/>
-      <c r="C25" s="21" t="s">
-        <v>5</v>
-      </c>
+      <c r="C25" s="21"/>
       <c r="D25" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3786,12 +3643,10 @@
       <c r="S25" s="10"/>
       <c r="T25" s="8"/>
     </row>
-    <row r="26" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:20" ht="13.5" customHeight="1">
       <c r="A26" s="87"/>
       <c r="B26" s="38"/>
-      <c r="C26" s="21" t="s">
-        <v>3</v>
-      </c>
+      <c r="C26" s="21"/>
       <c r="D26" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3831,12 +3686,10 @@
       <c r="S26" s="10"/>
       <c r="T26" s="8"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20">
       <c r="A27" s="1"/>
       <c r="B27" s="38"/>
-      <c r="C27" s="23" t="s">
-        <v>5</v>
-      </c>
+      <c r="C27" s="23"/>
       <c r="D27" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3876,12 +3729,10 @@
       <c r="S27" s="10"/>
       <c r="T27" s="8"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20">
       <c r="A28" s="1"/>
       <c r="B28" s="38"/>
-      <c r="C28" s="23" t="s">
-        <v>5</v>
-      </c>
+      <c r="C28" s="23"/>
       <c r="D28" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3921,12 +3772,10 @@
       <c r="S28" s="10"/>
       <c r="T28" s="8"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20">
       <c r="A29" s="1"/>
       <c r="B29" s="38"/>
-      <c r="C29" s="23" t="s">
-        <v>5</v>
-      </c>
+      <c r="C29" s="23"/>
       <c r="D29" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3966,12 +3815,10 @@
       <c r="S29" s="10"/>
       <c r="T29" s="8"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20">
       <c r="A30" s="20"/>
       <c r="B30" s="38"/>
-      <c r="C30" s="23" t="s">
-        <v>1</v>
-      </c>
+      <c r="C30" s="23"/>
       <c r="D30" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4011,12 +3858,10 @@
       <c r="S30" s="10"/>
       <c r="T30" s="8"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20">
       <c r="A31" s="77"/>
       <c r="B31" s="46"/>
-      <c r="C31" s="78" t="s">
-        <v>1</v>
-      </c>
+      <c r="C31" s="78"/>
       <c r="D31" s="88">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4123,11 +3968,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="27.875" customWidth="1"/>
     <col min="2" max="2" width="33.375" customWidth="1"/>
@@ -4135,134 +3980,134 @@
     <col min="4" max="4" width="29.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="105"/>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="18.75">
+      <c r="A1" s="106"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="25"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="26"/>
       <c r="B3" s="27"/>
       <c r="C3" s="28"/>
       <c r="D3" s="29"/>
       <c r="E3" s="27"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" s="26"/>
       <c r="B4" s="27"/>
       <c r="C4" s="28"/>
       <c r="D4" s="29"/>
       <c r="E4" s="27"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="26"/>
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
       <c r="D5" s="29"/>
       <c r="E5" s="27"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="26"/>
       <c r="B6" s="27"/>
       <c r="C6" s="28"/>
       <c r="D6" s="29"/>
       <c r="E6" s="27"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="26"/>
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
       <c r="D7" s="29"/>
       <c r="E7" s="27"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="26"/>
       <c r="B8" s="27"/>
       <c r="C8" s="28"/>
       <c r="D8" s="29"/>
       <c r="E8" s="27"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="26"/>
       <c r="B9" s="27"/>
       <c r="C9" s="28"/>
       <c r="D9" s="29"/>
       <c r="E9" s="27"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="26"/>
       <c r="B10" s="27"/>
       <c r="C10" s="28"/>
       <c r="D10" s="29"/>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="16.5">
       <c r="A11" s="26"/>
       <c r="B11" s="31"/>
       <c r="C11" s="28"/>
       <c r="D11" s="32"/>
       <c r="E11" s="27"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="26"/>
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
       <c r="D12" s="29"/>
       <c r="E12" s="27"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="26"/>
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
       <c r="E13" s="27"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14" s="26"/>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
       <c r="D14" s="29"/>
       <c r="E14" s="27"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="107" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="107" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="107" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="107" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="107" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="107" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="107" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="107" t="s">
-        <v>107</v>
+    <row r="18" spans="1:2">
+      <c r="A18" s="92" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="92" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="92" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="92" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="92" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="92" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -4283,9 +4128,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4293,27 +4138,27 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:4">
       <c r="D2">
         <f>A2+B2+C2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="C4" s="37" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>